<commit_message>
Machine Learning Operations tasks
</commit_message>
<xml_diff>
--- a/02. Machine Learning Operations/checklist-azureml-pipelilne.xlsx
+++ b/02. Machine Learning Operations/checklist-azureml-pipelilne.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelbryanlaricobarzola/Documents/capacitaciones/udacity-machine-learning-azure/Machine-Learning-Engineering-Azure/02. Machine Learning Operations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76896F19-A1C2-D740-A356-DBF84C02C76F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D0402A-B8C5-3742-A459-D5B16CC85EA2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="18420" windowHeight="19100" xr2:uid="{F10E88EA-E29C-C840-A4B7-F93F6596BFB0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19100" activeTab="1" xr2:uid="{F10E88EA-E29C-C840-A4B7-F93F6596BFB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
+    <sheet name="Project" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,8 +30,51 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{2BF97484-40F5-9042-8F9A-F7EF92C3FE52}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Toma sus 30 minutos aproximadamente.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>Iniciallizar el workspace</t>
   </si>
@@ -145,15 +189,98 @@
   <si>
     <t>Machine Learning Pipeline con AutoMLStep</t>
   </si>
+  <si>
+    <t>metrics_output = pipeline_run.get_pipeline_output(metrics_output_name)
+num_file_downloaded = metrics_output.download('.', show_progress=True)
+with open(metrics_output._path_on_datastore) as f:
+    metrics_output_result = f.read()
+deserialized_metrics_output = json.loads(metrics_output_result)
+df = pd.DataFrame(deserialized_metrics_output)
+df</t>
+  </si>
+  <si>
+    <t>best_model_output = pipeline_run.get_pipeline_output(best_model_output_name)
+num_file_downloaded = best_model_output.download('.', show_progress=True)</t>
+  </si>
+  <si>
+    <t>published_pipeline = pipeline_run.publish_pipeline(
+    name="Bikesharing Train", description="Training bikesharing pipeline", version="1.0")
+published_pipeline</t>
+  </si>
+  <si>
+    <t>rest_endpoint = published_pipeline.endpoint
+response = requests.post(rest_endpoint, 
+                         headers=auth_header, 
+                         json={"ExperimentName": "pipeline-bike-rest-endpoint"}
+                        )</t>
+  </si>
+  <si>
+    <t>Evaluar los resultados</t>
+  </si>
+  <si>
+    <t>try:
+    response.raise_for_status()
+except Exception:    
+    raise Exception("Received bad response from the endpoint: {}\n"
+                    "Response Code: {}\n"
+                    "Headers: {}\n"
+                    "Content: {}".format(rest_endpoint, response.status_code, response.headers, response.content))
+run_id = response.json().get('Id')
+print('Submitted pipeline run: ', run_id)</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Authentication</t>
+  </si>
+  <si>
+    <t>Automated ML Experiment</t>
+  </si>
+  <si>
+    <t>Deploy the best model</t>
+  </si>
+  <si>
+    <t>Enable logging</t>
+  </si>
+  <si>
+    <t>Swagger Documentation</t>
+  </si>
+  <si>
+    <t>Consume model endpoints</t>
+  </si>
+  <si>
+    <t>Create and pusblish a pipeline</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -173,8 +300,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,6 +324,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -200,18 +352,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -227,6 +382,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85248AEC-9144-9B46-BCF8-86B31D4AB810}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4292600" y="406400"/>
+          <a:ext cx="5435600" cy="2717800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -525,11 +729,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0688EEC-518D-6B44-838C-7445C24C0CB9}">
-  <dimension ref="A2:B17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0688EEC-518D-6B44-838C-7445C24C0CB9}">
+  <dimension ref="A2:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -624,34 +828,142 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="153" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="85" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="187" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C44609B4-CB8A-4C4F-9455-B1EF90BE0CE1}">
+  <dimension ref="B5:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>